<commit_message>
Various updates, including latest Altium files
</commit_message>
<xml_diff>
--- a/schematic/OpenStrom - BOM.xlsx
+++ b/schematic/OpenStrom - BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias E. Zeitler\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias E. Zeitler\Documents\Business\Open Strom\Github\openstrom\schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>#</t>
   </si>
@@ -231,12 +231,6 @@
     <t>http://www.hktdc.com/suppliers-products/High-Power-Relay/en/1X06TH7E/2984390/</t>
   </si>
   <si>
-    <t>$0,70</t>
-  </si>
-  <si>
-    <t>7.00</t>
-  </si>
-  <si>
     <t>Ordering info:BT90-SS-05-D-M</t>
   </si>
 </sst>
@@ -245,8 +239,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="##0"/>
-    <numFmt numFmtId="173" formatCode="[$$]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="##0"/>
+    <numFmt numFmtId="165" formatCode="[$$]#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -316,30 +310,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -901,7 +895,7 @@
   <dimension ref="A1:IV974"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="A17:IV17"/>
+      <selection activeCell="B1" sqref="B1:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3465,14 +3459,15 @@
       <c r="F16">
         <v>10</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="H16" s="13">
+        <f>F16*G16</f>
+        <v>7</v>
+      </c>
+      <c r="I16" t="s">
         <v>70</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" t="s">
-        <v>72</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>69</v>

</xml_diff>